<commit_message>
Hide in the Shadows, Shadow Cloak, Shadowstep fix
</commit_message>
<xml_diff>
--- a/Thief Character Card Stats.xlsx
+++ b/Thief Character Card Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Stuff\Coding\ModdingSlayTheSpire\my_mods\git\StS-TheThiefMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDFDE67-2FE5-465F-9B7F-A3DA598C181E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086B5701-C46F-40F9-AD50-4EA5417C106A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="278" xr2:uid="{AD2E1A73-3376-4E41-A344-6779F4DBBFBB}"/>
   </bookViews>
@@ -414,12 +414,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -439,6 +433,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -476,18 +482,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -550,12 +544,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -575,6 +563,24 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -591,12 +597,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -858,18 +858,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FF4810EE-C708-4E37-835D-7BB9DD96E48C}" name="Column1" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{4B7223C6-8335-433A-9378-28EFCCDBF04D}" name="Silent" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{2C581A80-D6F5-4915-9D06-BA8D353C068D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{BA528A4A-ED02-4115-906A-32084823D809}" name="Defect" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{FA953889-5C20-4CA7-8F3C-AA6F43A0A33C}" name="Thief" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{FF4810EE-C708-4E37-835D-7BB9DD96E48C}" name="Column1" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{4B7223C6-8335-433A-9378-28EFCCDBF04D}" name="Silent" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{2C581A80-D6F5-4915-9D06-BA8D353C068D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="31" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{BA528A4A-ED02-4115-906A-32084823D809}" name="Defect" totalsRowFunction="sum" dataDxfId="30" totalsRowDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{FA953889-5C20-4CA7-8F3C-AA6F43A0A33C}" name="Thief" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53B8ADF9-4707-47E1-BDFA-3F006EA823AB}" name="Table24" displayName="Table24" ref="G7:K12" totalsRowCount="1" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53B8ADF9-4707-47E1-BDFA-3F006EA823AB}" name="Table24" displayName="Table24" ref="G7:K12" totalsRowCount="1" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="G7:K11" xr:uid="{CE12703D-A0E8-4EAA-9688-E5928D5B5BFB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -878,18 +878,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{28832C6B-C5A0-4B28-9B43-B972B39FC7E3}" name="Column1" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{BBDEB0D6-F456-42CF-9E45-0769D86C8EBC}" name="Silent" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{FE11044C-0B04-4341-B805-DD3FC475A98D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{3473F5BA-E9A0-42BC-A801-C0AA1A01137A}" name="Defect" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{706E8FB7-3FE6-4437-8FE5-F955111BE534}" name="Thief" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{28832C6B-C5A0-4B28-9B43-B972B39FC7E3}" name="Column1" totalsRowLabel="Total" dataDxfId="26" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{BBDEB0D6-F456-42CF-9E45-0769D86C8EBC}" name="Silent" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{FE11044C-0B04-4341-B805-DD3FC475A98D}" name="Ironclad" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3473F5BA-E9A0-42BC-A801-C0AA1A01137A}" name="Defect" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{706E8FB7-3FE6-4437-8FE5-F955111BE534}" name="Thief" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C72900FD-3D9E-415B-8DD8-AF9885345991}" name="Table245" displayName="Table245" ref="G18:K22" totalsRowCount="1" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C72900FD-3D9E-415B-8DD8-AF9885345991}" name="Table245" displayName="Table245" ref="G18:K22" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="G18:K21" xr:uid="{B83B401D-8396-4C3C-8AF6-1D22A1900080}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -898,11 +898,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{48FFD4D9-93EC-4372-BA8E-DF53D2155AA8}" name="Column1" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B001FE0B-0A93-4138-837A-59C8A8D0B15D}" name="Silent" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{75DCC043-06AD-429B-BFF7-47F0588947D4}" name="Ironclad" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{A35EFF12-81B8-49BF-8505-BAA7346C7660}" name="Defect" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{794D68DF-FC01-46E7-BC8F-41362EBFA07B}" name="Thief" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{48FFD4D9-93EC-4372-BA8E-DF53D2155AA8}" name="Column1" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{B001FE0B-0A93-4138-837A-59C8A8D0B15D}" name="Silent" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{75DCC043-06AD-429B-BFF7-47F0588947D4}" name="Ironclad" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A35EFF12-81B8-49BF-8505-BAA7346C7660}" name="Defect" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{794D68DF-FC01-46E7-BC8F-41362EBFA07B}" name="Thief" totalsRowFunction="count" dataDxfId="11" totalsRowDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Gremy Simple Dark" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1205,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7173905A-9702-4724-9D18-DFCD7AC58563}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1216,7 @@
     <col min="1" max="16384" width="12.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>12</v>
       </c>
@@ -1227,7 +1227,7 @@
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -1236,7 +1236,7 @@
       <c r="F2" s="28"/>
       <c r="G2" s="28"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -1245,7 +1245,7 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
         <v>5</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="J6" s="27"/>
       <c r="K6" s="27"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>0</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>43</v>
       </c>
       <c r="E9" s="4">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="6" t="s">
@@ -1373,10 +1373,10 @@
         <v>18</v>
       </c>
       <c r="K9" s="4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>2</v>
       </c>
@@ -1406,10 +1406,10 @@
         <v>36</v>
       </c>
       <c r="K10" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -1474,10 +1474,10 @@
       </c>
       <c r="K12" s="5">
         <f>SUBTOTAL(109,Table24[Thief])</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1495,22 +1495,18 @@
       </c>
       <c r="E13" s="5">
         <f>SUBTOTAL(109,Table2[Thief])</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
       <c r="D15" s="28"/>
-      <c r="N15" s="4">
-        <f>75-12</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="28"/>
       <c r="C16" s="28"/>

</xml_diff>